<commit_message>
Changed TestData spreadsheet and optimized Registration Page a lpt
</commit_message>
<xml_diff>
--- a/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayyanar\eclipse-workspace\MyLotto\src\main\java\com\mylotto\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0008171D-FF2F-4EC1-8995-28406901091B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC7E6C7-8F8B-43B8-89AF-2E601C50A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t>email</t>
   </si>
@@ -65,13 +65,97 @@
   </si>
   <si>
     <t>a.subbu1984@gmail.com</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>dob_date</t>
+  </si>
+  <si>
+    <t>dob_year</t>
+  </si>
+  <si>
+    <t>Subramani</t>
+  </si>
+  <si>
+    <t>`1963</t>
+  </si>
+  <si>
+    <t>`1964</t>
+  </si>
+  <si>
+    <t>4123321</t>
+  </si>
+  <si>
+    <t>441224</t>
+  </si>
+  <si>
+    <t>a.subbu1988@gmail.com</t>
+  </si>
+  <si>
+    <t>a.subbu1989@gmail.com</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>Mitchel</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>`1965</t>
+  </si>
+  <si>
+    <t>`1966</t>
+  </si>
+  <si>
+    <t>`1967</t>
+  </si>
+  <si>
+    <t>441225</t>
+  </si>
+  <si>
+    <t>441226</t>
+  </si>
+  <si>
+    <t>441227</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +167,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,9 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -393,21 +485,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,52 +517,159 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1578B7F5-D39E-43EC-B466-F3456FF06A76}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{8666E99C-793A-4E9B-A1D5-AFC682490A1A}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{20023218-5D14-40D2-B48C-0F46FD59C904}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{E6CBEBD6-8AF5-489C-B209-5D22DE1DD2CD}"/>
-    <hyperlink ref="A2:A3" r:id="rId5" display="a.subbu1987@gmail.com" xr:uid="{C8AF4A28-D932-406E-978B-D949FCA3D9BA}"/>
-    <hyperlink ref="A2" r:id="rId6" xr:uid="{395CD5E9-6804-4EB5-B302-5F24C92F5ACB}"/>
-    <hyperlink ref="A3" r:id="rId7" xr:uid="{D39F6C98-EA79-46F5-A6E1-234446E1A7B4}"/>
+    <hyperlink ref="A2:A3" r:id="rId1" display="a.subbu1987@gmail.com" xr:uid="{C8AF4A28-D932-406E-978B-D949FCA3D9BA}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{395CD5E9-6804-4EB5-B302-5F24C92F5ACB}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D39F6C98-EA79-46F5-A6E1-234446E1A7B4}"/>
+    <hyperlink ref="A4:A6" r:id="rId4" display="a.subbu1987@gmail.com" xr:uid="{F2572CCB-2428-4535-A198-F6E68FD82FC9}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{85D0765B-9B74-42D5-9740-A644DD2CF592}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{BF9513A9-FDAB-4058-AEF8-3C143D0A3BA1}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{4098CD04-E4A4-45C3-9A1D-EF71B95726D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed xpath in Reg java
</commit_message>
<xml_diff>
--- a/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayyanar\eclipse-workspace\MyLotto\src\main\java\com\mylotto\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC7E6C7-8F8B-43B8-89AF-2E601C50A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B36EA0-A400-4ED6-B9A5-048C11E25DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33930" yWindow="1290" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" r:id="rId1"/>
     <sheet name="Players" sheetId="2" r:id="rId2"/>
+    <sheet name="Temp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="41">
   <si>
     <t>email</t>
   </si>
@@ -485,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,123 +554,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2:A3" r:id="rId1" display="a.subbu1987@gmail.com" xr:uid="{C8AF4A28-D932-406E-978B-D949FCA3D9BA}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{395CD5E9-6804-4EB5-B302-5F24C92F5ACB}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{D39F6C98-EA79-46F5-A6E1-234446E1A7B4}"/>
-    <hyperlink ref="A4:A6" r:id="rId4" display="a.subbu1987@gmail.com" xr:uid="{F2572CCB-2428-4535-A198-F6E68FD82FC9}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{85D0765B-9B74-42D5-9740-A644DD2CF592}"/>
-    <hyperlink ref="A5" r:id="rId6" xr:uid="{BF9513A9-FDAB-4058-AEF8-3C143D0A3BA1}"/>
-    <hyperlink ref="A6" r:id="rId7" xr:uid="{4098CD04-E4A4-45C3-9A1D-EF71B95726D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -989,4 +881,192 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCD1A0E-B64E-4F75-BCE5-E9394875E1E4}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2:A3" r:id="rId1" display="a.subbu1987@gmail.com" xr:uid="{95F3B5D4-64C4-4F33-8C5A-F8C78E7F7FCB}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{2CEBD04E-8CA5-4772-AFD4-5DFD0EF49546}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{63DDB5FB-019E-42D4-8523-EAE40F27E8AA}"/>
+    <hyperlink ref="A4:A6" r:id="rId4" display="a.subbu1987@gmail.com" xr:uid="{D063C4B3-2AD3-4178-B85F-ED6425506326}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{8F3EFF56-B8DA-4340-8A92-1ABA6639FC6E}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{B0269EC5-F357-4D04-8177-B71EED8368C3}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{4200FED4-B12C-4943-94A3-62DDFC2ACE0E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Included Lotto Dips java
</commit_message>
<xml_diff>
--- a/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayyanar\eclipse-workspace\MyLotto\src\main\java\com\mylotto\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B36EA0-A400-4ED6-B9A5-048C11E25DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6A560-6467-46F9-97B5-96E2B7CDC7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33930" yWindow="1290" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" r:id="rId1"/>
     <sheet name="Players" sheetId="2" r:id="rId2"/>
-    <sheet name="Temp" sheetId="3" r:id="rId3"/>
+    <sheet name="Lotto" sheetId="4" r:id="rId3"/>
+    <sheet name="Temp" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>email</t>
   </si>
@@ -44,27 +45,15 @@
     <t>cpassword</t>
   </si>
   <si>
-    <t>a.subbu1985@gmail.com</t>
-  </si>
-  <si>
-    <t>Subbu</t>
-  </si>
-  <si>
     <t>Ayyanar</t>
   </si>
   <si>
-    <t>Shreya@1</t>
-  </si>
-  <si>
     <t>a.subbu1986@gmail.com</t>
   </si>
   <si>
     <t>a.subbu1987@gmail.com</t>
   </si>
   <si>
-    <t>SubbuA</t>
-  </si>
-  <si>
     <t>a.subbu1984@gmail.com</t>
   </si>
   <si>
@@ -150,6 +139,18 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>player_email</t>
+  </si>
+  <si>
+    <t>player_password</t>
+  </si>
+  <si>
+    <t>a.robinson@xtra.co.nz</t>
+  </si>
+  <si>
+    <t>brookswhanau@xtra.co.nz</t>
   </si>
 </sst>
 </file>
@@ -488,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,39 +520,39 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -567,323 +568,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0263B022-E60E-4E3D-8414-11F3561B4CE0}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{359A92D4-A622-4801-A411-01FB2225BEA8}"/>
-    <hyperlink ref="E1" r:id="rId2" xr:uid="{11775819-A69B-44D1-899C-625007BD1EBB}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{1C457637-615F-44EA-8B01-991CD83E68B2}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{37657332-5587-437B-B9AD-100366716CC5}"/>
-    <hyperlink ref="A3" r:id="rId5" xr:uid="{F95AED39-E3F8-496D-9E10-394E90204A9D}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{A55168A2-BA61-43C3-820F-B07F94AFA18B}"/>
-    <hyperlink ref="E3" r:id="rId7" xr:uid="{3EC42C8F-7CB0-45CF-9B91-8F72B1A24654}"/>
-    <hyperlink ref="A4" r:id="rId8" xr:uid="{C6F74439-F4F6-461F-ACB2-CB595EB9DE38}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{8EC10D96-2D5F-43F8-B8AC-C2EFC5F5D8F8}"/>
-    <hyperlink ref="E4" r:id="rId10" xr:uid="{63ED3809-CE50-465C-A80D-6C4F498081A0}"/>
-    <hyperlink ref="A5" r:id="rId11" xr:uid="{BE7E41F5-BC98-45A2-8DD4-8FB1DFB9884C}"/>
-    <hyperlink ref="D5" r:id="rId12" xr:uid="{8248F5EB-3BDB-4FE1-946F-C5D0219E1F20}"/>
-    <hyperlink ref="E5" r:id="rId13" xr:uid="{33081699-8B48-4B39-8AB7-60501E5E16B5}"/>
-    <hyperlink ref="A6" r:id="rId14" xr:uid="{B7DFBF49-BC2E-486B-8477-7C1C5E181A53}"/>
-    <hyperlink ref="D6" r:id="rId15" xr:uid="{32CB8D2B-B311-43AE-9B88-7C4C0F0DAAF7}"/>
-    <hyperlink ref="E6" r:id="rId16" xr:uid="{FB60EEC4-69FF-481B-82E0-49BDF7151773}"/>
-    <hyperlink ref="A7" r:id="rId17" xr:uid="{685D18E7-D25D-4089-B737-027370C47FB9}"/>
-    <hyperlink ref="D7" r:id="rId18" xr:uid="{AC87122A-27BC-482A-BC1E-542DDE695E68}"/>
-    <hyperlink ref="E7" r:id="rId19" xr:uid="{4A9BF85D-525D-4641-8190-1966B68B081A}"/>
-    <hyperlink ref="A8" r:id="rId20" xr:uid="{2651D644-7B40-4690-8423-8BFFCB22BF42}"/>
-    <hyperlink ref="D8" r:id="rId21" xr:uid="{E5553886-3D50-41E7-89C1-A38EC9294C7C}"/>
-    <hyperlink ref="E8" r:id="rId22" xr:uid="{E0C8670E-AEAE-4CBC-ACC6-66D184882344}"/>
-    <hyperlink ref="A9" r:id="rId23" xr:uid="{1F278E2E-481D-4FE2-9E94-F3A0A84DC938}"/>
-    <hyperlink ref="D9" r:id="rId24" xr:uid="{5C94C8AA-2FD3-4875-913B-4978A43C63EA}"/>
-    <hyperlink ref="E9" r:id="rId25" xr:uid="{A1594BD8-30AA-4471-BFF1-737E11ABC3C8}"/>
-    <hyperlink ref="A10" r:id="rId26" xr:uid="{88198B0A-5CBF-4DB3-BED0-BA668AFB97A6}"/>
-    <hyperlink ref="D10" r:id="rId27" xr:uid="{7E087C07-A673-492E-8235-23EBFB339EEA}"/>
-    <hyperlink ref="E10" r:id="rId28" xr:uid="{8EDAEB7F-F884-4109-8AE3-AB6AF6EE2390}"/>
-    <hyperlink ref="A11" r:id="rId29" xr:uid="{25E51E98-F374-4D5D-A34A-036BC8CC63B5}"/>
-    <hyperlink ref="D11" r:id="rId30" xr:uid="{7ED62587-167B-40A4-8CE5-B66C34212FFA}"/>
-    <hyperlink ref="E11" r:id="rId31" xr:uid="{6CBDB587-E246-4DF0-8DF4-6D730115BBEB}"/>
-    <hyperlink ref="A12" r:id="rId32" xr:uid="{71BC94DE-0E1A-4367-B949-5FED82E40A5A}"/>
-    <hyperlink ref="D12" r:id="rId33" xr:uid="{982C5866-753B-4BB7-93F5-56678D243736}"/>
-    <hyperlink ref="E12" r:id="rId34" xr:uid="{668010E9-C82B-4E95-AC53-8F06DAEE24C3}"/>
-    <hyperlink ref="A13" r:id="rId35" xr:uid="{73ADC327-9817-445F-AAC0-E22FDD0B6C43}"/>
-    <hyperlink ref="D13" r:id="rId36" xr:uid="{18C9CF8D-1333-4C57-BA57-85F9F41B6388}"/>
-    <hyperlink ref="E13" r:id="rId37" xr:uid="{75DE29E7-03BF-41D7-8162-386F5B7CF643}"/>
-    <hyperlink ref="A14" r:id="rId38" xr:uid="{1EA68D9F-5FD5-43FF-A685-40ACF26A6F39}"/>
-    <hyperlink ref="D14" r:id="rId39" xr:uid="{8C400EDD-AEE1-4084-B813-7A17F682725A}"/>
-    <hyperlink ref="E14" r:id="rId40" xr:uid="{A90FF13C-07C6-4760-B1C2-1DFD8BC865FC}"/>
-    <hyperlink ref="A15" r:id="rId41" xr:uid="{250E6458-315B-4E64-83BF-A08366E194C6}"/>
-    <hyperlink ref="D15" r:id="rId42" xr:uid="{B88240BB-8BA5-41FD-932E-96CB6E585377}"/>
-    <hyperlink ref="E15" r:id="rId43" xr:uid="{976EBEDD-5AF6-47C4-8F14-3ADF0B2C3586}"/>
-    <hyperlink ref="A1:A2" r:id="rId44" display="a.subbu1987@gmail.com" xr:uid="{34801F06-47FD-4493-B88C-F443AC9E4722}"/>
-    <hyperlink ref="A1" r:id="rId45" xr:uid="{BBE36620-4F73-4939-9857-71C70C445ECE}"/>
-    <hyperlink ref="A2" r:id="rId46" xr:uid="{7F6736D1-BD11-4740-B937-A372A101633E}"/>
+    <hyperlink ref="A2" r:id="rId1" display="a.subbu1987@gmail.com" xr:uid="{BE3F2F2F-660F-4007-82FF-438B46D21120}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{CF21E178-C3AB-4535-86DE-762B86C9A055}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92481A24-BD1B-4C7A-BC50-F18C069C75F3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCD1A0E-B64E-4F75-BCE5-E9394875E1E4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -918,143 +669,143 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included Email Activation code, IGT control access
</commit_message>
<xml_diff>
--- a/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/mylotto/qa/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayyanar\eclipse-workspace\MyLotto\src\main\java\com\mylotto\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6A560-6467-46F9-97B5-96E2B7CDC7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B90F5FC-F389-41C9-BF8C-F594C8FECB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-1950" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>email</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>brookswhanau@xtra.co.nz</t>
+  </si>
+  <si>
+    <t>4123322</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -487,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
@@ -530,8 +539,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -553,6 +562,32 @@
       </c>
       <c r="H2" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -560,9 +595,10 @@
   <hyperlinks>
     <hyperlink ref="A2:A3" r:id="rId1" display="a.subbu1987@gmail.com" xr:uid="{C8AF4A28-D932-406E-978B-D949FCA3D9BA}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{395CD5E9-6804-4EB5-B302-5F24C92F5ACB}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{85FDB962-00B5-4440-BE9F-FF67BA81BC15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -570,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0263B022-E60E-4E3D-8414-11F3561B4CE0}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>